<commit_message>
GuiClient icon, update product backlog
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="4245" windowWidth="15480" windowHeight="11640"/>
+    <workbookView xWindow="120" yWindow="4845" windowWidth="15480" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -131,7 +131,13 @@
     <t>Der User kann  über Mikrofon kommunizieren.</t>
   </si>
   <si>
-    <t>diverse Bugfixes</t>
+    <t>diverse bugfixes</t>
+  </si>
+  <si>
+    <t>Der User kann vergangene Verbindungen sehen.</t>
+  </si>
+  <si>
+    <t>Der User kann ein Icon sehen.</t>
   </si>
 </sst>
 </file>
@@ -622,8 +628,8 @@
   <dimension ref="A1:XFD84"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
+      <pane ySplit="5" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33785,20 +33791,30 @@
       <c r="D22" s="26">
         <v>42282</v>
       </c>
-      <c r="E22" s="26"/>
-      <c r="F22" s="23"/>
+      <c r="E22" s="26">
+        <v>42328</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>35</v>
+      </c>
       <c r="G22" s="23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H22" s="23"/>
     </row>
     <row r="23" spans="1:8" s="24" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22"/>
       <c r="B23" s="23"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="26"/>
+      <c r="D23" s="26">
+        <v>42282</v>
+      </c>
+      <c r="E23" s="26">
+        <v>42328</v>
+      </c>
       <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="23" t="s">
+        <v>37</v>
+      </c>
       <c r="H23" s="23"/>
     </row>
     <row r="24" spans="1:8" s="24" customFormat="1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>